<commit_message>
balanced the triplets. saved screenshots
</commit_message>
<xml_diff>
--- a/docs/choosing_triplets_new_range.xlsx
+++ b/docs/choosing_triplets_new_range.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="17">
   <si>
     <t>simulation name</t>
   </si>
@@ -86,6 +86,9 @@
   <si>
     <t xml:space="preserve">step_size </t>
   </si>
+  <si>
+    <t>balancing</t>
+  </si>
 </sst>
 </file>
 
@@ -100,7 +103,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +113,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -135,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -171,6 +222,60 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,8 +559,8 @@
   <dimension ref="A1:L94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29:A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,15 +618,15 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="15">
         <f>E2-F2</f>
         <v>8</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="15">
         <f>E2-G2</f>
         <v>-8</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="16">
         <f>F2-G2</f>
         <v>-16</v>
       </c>
@@ -559,15 +664,15 @@
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="15">
         <f t="shared" ref="B3:B28" si="0">E3-F3</f>
         <v>8</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="15">
         <f t="shared" ref="C3:C28" si="1">E3-G3</f>
         <v>-8</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="16">
         <f t="shared" ref="D3:D28" si="2">F3-G3</f>
         <v>-16</v>
       </c>
@@ -605,28 +710,28 @@
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="15">
         <f t="shared" si="1"/>
         <v>-8</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="16">
         <f t="shared" si="2"/>
         <v>-16</v>
       </c>
       <c r="E4" s="5">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F4" s="13">
         <f>E4-Sheet2!$B$1</f>
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="G4" s="13">
         <f>E4+Sheet2!$B$1</f>
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="3"/>
@@ -651,15 +756,15 @@
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="17">
         <f t="shared" si="1"/>
         <v>-16</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="18">
         <f t="shared" si="2"/>
         <v>-32</v>
       </c>
@@ -697,15 +802,15 @@
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="17">
         <f t="shared" si="1"/>
         <v>-16</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="18">
         <f t="shared" si="2"/>
         <v>-32</v>
       </c>
@@ -743,28 +848,28 @@
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="17">
         <f t="shared" si="1"/>
         <v>-16</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="18">
         <f t="shared" si="2"/>
         <v>-32</v>
       </c>
       <c r="E7" s="5">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F7" s="13">
         <f>E7-Sheet2!$B$1*2</f>
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G7" s="13">
         <f>E7+Sheet2!$B$1*2</f>
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="3"/>
@@ -789,15 +894,15 @@
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="19">
         <f t="shared" ref="B8" si="6">E8-F8</f>
         <v>24</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="19">
         <f t="shared" ref="C8" si="7">E8-G8</f>
         <v>-24</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="20">
         <f t="shared" ref="D8" si="8">F8-G8</f>
         <v>-48</v>
       </c>
@@ -835,15 +940,15 @@
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="19">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="19">
         <f t="shared" si="1"/>
         <v>-24</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="20">
         <f t="shared" si="2"/>
         <v>-48</v>
       </c>
@@ -881,28 +986,28 @@
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="19">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="19">
         <f t="shared" si="1"/>
         <v>-24</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="20">
         <f t="shared" si="2"/>
         <v>-48</v>
       </c>
       <c r="E10" s="5">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F10" s="13">
         <f>E10-Sheet2!$B$1*3</f>
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G10" s="13">
         <f>E10+Sheet2!$B$1*3</f>
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="3"/>
@@ -927,28 +1032,28 @@
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="21">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="21">
         <f t="shared" si="1"/>
         <v>-16</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="22">
         <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="E11" s="5">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F11" s="13">
         <f>E11-Sheet2!$B$1*1</f>
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G11" s="13">
         <f>E11+Sheet2!$B$1*2</f>
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="3"/>
@@ -973,15 +1078,15 @@
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="21">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="21">
         <f t="shared" si="1"/>
         <v>-16</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="22">
         <f t="shared" si="2"/>
         <v>-24</v>
       </c>
@@ -1019,28 +1124,28 @@
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="21">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="21">
         <f t="shared" si="1"/>
         <v>-16</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="22">
         <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="E13" s="5">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F13" s="13">
         <f>E13-Sheet2!$B$1*1</f>
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G13" s="13">
         <f>E13+Sheet2!$B$1*2</f>
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="3"/>
@@ -1065,15 +1170,15 @@
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="23">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="23">
         <f t="shared" si="1"/>
         <v>-8</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="24">
         <f t="shared" si="2"/>
         <v>-24</v>
       </c>
@@ -1111,15 +1216,15 @@
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="23">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="23">
         <f t="shared" si="1"/>
         <v>-8</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="24">
         <f t="shared" si="2"/>
         <v>-24</v>
       </c>
@@ -1157,28 +1262,28 @@
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="23">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="23">
         <f t="shared" si="1"/>
         <v>-8</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="24">
         <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="E16" s="5">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F16" s="13">
         <f>E16-Sheet2!$B$1*2</f>
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="G16" s="13">
         <f>E16+Sheet2!$B$1*1</f>
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="3"/>
@@ -1203,15 +1308,15 @@
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="25">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="25">
         <f t="shared" si="1"/>
         <v>-24</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="26">
         <f t="shared" si="2"/>
         <v>-40</v>
       </c>
@@ -1249,15 +1354,15 @@
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="25">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="25">
         <f t="shared" si="1"/>
         <v>-24</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="26">
         <f t="shared" si="2"/>
         <v>-40</v>
       </c>
@@ -1295,28 +1400,28 @@
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="25">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="25">
         <f t="shared" si="1"/>
         <v>-24</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="26">
         <f t="shared" si="2"/>
         <v>-40</v>
       </c>
       <c r="E19" s="5">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F19" s="13">
         <f>E19-Sheet2!$B$1*2</f>
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G19" s="13">
         <f>E19+Sheet2!$B$1*3</f>
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H19" s="5">
         <f t="shared" si="3"/>
@@ -1341,28 +1446,28 @@
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="27">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="27">
         <f t="shared" si="1"/>
         <v>-16</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="28">
         <f t="shared" si="2"/>
         <v>-40</v>
       </c>
       <c r="E20" s="5">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F20" s="13">
         <f>E20-Sheet2!$B$1*3</f>
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G20" s="13">
         <f>E20+Sheet2!$B$1*2</f>
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="H20" s="5">
         <f t="shared" si="3"/>
@@ -1387,15 +1492,15 @@
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="27">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="27">
         <f t="shared" si="1"/>
         <v>-16</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="28">
         <f t="shared" si="2"/>
         <v>-40</v>
       </c>
@@ -1433,28 +1538,28 @@
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="27">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="27">
         <f t="shared" si="1"/>
         <v>-16</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="28">
         <f t="shared" si="2"/>
         <v>-40</v>
       </c>
       <c r="E22" s="5">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F22" s="13">
         <f>E22-Sheet2!$B$1*3</f>
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G22" s="13">
         <f>E22+Sheet2!$B$1*2</f>
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H22" s="5">
         <f t="shared" si="3"/>
@@ -1479,15 +1584,15 @@
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="29">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="29">
         <f t="shared" si="1"/>
         <v>-24</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="30">
         <f t="shared" si="2"/>
         <v>-32</v>
       </c>
@@ -1525,15 +1630,15 @@
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="29">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="29">
         <f t="shared" si="1"/>
         <v>-24</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="30">
         <f t="shared" si="2"/>
         <v>-32</v>
       </c>
@@ -1571,28 +1676,28 @@
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="29">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="29">
         <f t="shared" si="1"/>
         <v>-24</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="30">
         <f t="shared" si="2"/>
         <v>-32</v>
       </c>
       <c r="E25" s="5">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F25" s="13">
         <f>E25-Sheet2!$B$1*1</f>
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="G25" s="13">
         <f>E25+Sheet2!$B$1*3</f>
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="H25" s="5">
         <f t="shared" si="3"/>
@@ -1617,15 +1722,15 @@
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="31">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="31">
         <f t="shared" si="1"/>
         <v>-8</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="32">
         <f t="shared" si="2"/>
         <v>-32</v>
       </c>
@@ -1663,15 +1768,15 @@
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="31">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="31">
         <f t="shared" si="1"/>
         <v>-8</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="32">
         <f t="shared" si="2"/>
         <v>-32</v>
       </c>
@@ -1709,15 +1814,15 @@
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="31">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="31">
         <f t="shared" si="1"/>
         <v>-8</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="32">
         <f t="shared" si="2"/>
         <v>-32</v>
       </c>
@@ -1752,296 +1857,842 @@
       </c>
     </row>
     <row r="29" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="A29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="4">
+        <f t="shared" ref="B29:B30" si="12">E29-F29</f>
+        <v>8</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" ref="C29:C30" si="13">E29-G29</f>
+        <v>-74</v>
+      </c>
+      <c r="D29" s="5">
+        <f t="shared" ref="D29:D30" si="14">F29-G29</f>
+        <v>-82</v>
+      </c>
+      <c r="E29" s="4">
+        <v>38</v>
+      </c>
+      <c r="F29" s="4">
+        <v>30</v>
+      </c>
+      <c r="G29" s="4">
+        <v>112</v>
+      </c>
+      <c r="H29" s="5">
+        <f t="shared" ref="H29:H30" si="15">ABS(B29)</f>
+        <v>8</v>
+      </c>
+      <c r="I29" s="5">
+        <f t="shared" ref="I29:I30" si="16">ABS(C29)</f>
+        <v>74</v>
+      </c>
+      <c r="J29" s="5">
+        <f t="shared" ref="J29:J30" si="17">ABS(D29)</f>
+        <v>82</v>
+      </c>
       <c r="K29" s="8"/>
       <c r="L29" s="5"/>
     </row>
     <row r="30" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="A30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" si="13"/>
+        <v>-70</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" si="14"/>
+        <v>-78</v>
+      </c>
+      <c r="E30" s="4">
+        <v>46</v>
+      </c>
+      <c r="F30" s="4">
+        <v>38</v>
+      </c>
+      <c r="G30" s="4">
+        <v>116</v>
+      </c>
+      <c r="H30" s="5">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="I30" s="5">
+        <f t="shared" si="16"/>
+        <v>70</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" si="17"/>
+        <v>78</v>
+      </c>
       <c r="K30" s="8"/>
       <c r="L30" s="5"/>
     </row>
     <row r="31" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="A31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" ref="B31:B49" si="18">E31-F31</f>
+        <v>-18</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" ref="C31:C49" si="19">E31-G31</f>
+        <v>62</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" ref="D31:D49" si="20">F31-G31</f>
+        <v>80</v>
+      </c>
+      <c r="E31" s="4">
+        <v>100</v>
+      </c>
+      <c r="F31" s="4">
+        <v>118</v>
+      </c>
+      <c r="G31" s="4">
+        <v>38</v>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" ref="H31:H49" si="21">ABS(B31)</f>
+        <v>18</v>
+      </c>
+      <c r="I31" s="5">
+        <f t="shared" ref="I31:I49" si="22">ABS(C31)</f>
+        <v>62</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" ref="J31:J49" si="23">ABS(D31)</f>
+        <v>80</v>
+      </c>
       <c r="K31" s="8"/>
       <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
+      <c r="A32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="4">
+        <f t="shared" si="18"/>
+        <v>-8</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" si="19"/>
+        <v>8</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="20"/>
+        <v>16</v>
+      </c>
+      <c r="E32" s="4">
+        <v>108</v>
+      </c>
+      <c r="F32" s="4">
+        <v>116</v>
+      </c>
+      <c r="G32" s="4">
+        <v>100</v>
+      </c>
+      <c r="H32" s="4">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="I32" s="4">
+        <f t="shared" si="22"/>
+        <v>8</v>
+      </c>
+      <c r="J32" s="4">
+        <f t="shared" si="23"/>
+        <v>16</v>
+      </c>
       <c r="K32" s="8"/>
       <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
+      <c r="A33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="4">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" si="19"/>
+        <v>-8</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="20"/>
+        <v>-16</v>
+      </c>
+      <c r="E33" s="4">
+        <v>38</v>
+      </c>
+      <c r="F33" s="4">
+        <v>30</v>
+      </c>
+      <c r="G33" s="4">
+        <v>46</v>
+      </c>
+      <c r="H33" s="4">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="I33" s="4">
+        <f t="shared" si="22"/>
+        <v>8</v>
+      </c>
+      <c r="J33" s="4">
+        <f t="shared" si="23"/>
+        <v>16</v>
+      </c>
       <c r="K33" s="8"/>
       <c r="L33" s="5"/>
     </row>
     <row r="34" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
+      <c r="A34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="4">
+        <f t="shared" si="18"/>
+        <v>-16</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" si="19"/>
+        <v>64</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="20"/>
+        <v>80</v>
+      </c>
+      <c r="E34" s="4">
+        <v>94</v>
+      </c>
+      <c r="F34" s="4">
+        <v>110</v>
+      </c>
+      <c r="G34" s="4">
+        <v>30</v>
+      </c>
+      <c r="H34" s="4">
+        <f t="shared" si="21"/>
+        <v>16</v>
+      </c>
+      <c r="I34" s="4">
+        <f t="shared" si="22"/>
+        <v>64</v>
+      </c>
+      <c r="J34" s="4">
+        <f t="shared" si="23"/>
+        <v>80</v>
+      </c>
       <c r="K34" s="8"/>
       <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="A35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="4">
+        <f t="shared" si="18"/>
+        <v>32</v>
+      </c>
+      <c r="C35" s="4">
+        <f t="shared" si="19"/>
+        <v>-30</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="20"/>
+        <v>-62</v>
+      </c>
+      <c r="E35" s="4">
+        <v>62</v>
+      </c>
+      <c r="F35" s="4">
+        <v>30</v>
+      </c>
+      <c r="G35" s="4">
+        <v>92</v>
+      </c>
+      <c r="H35" s="4">
+        <f t="shared" si="21"/>
+        <v>32</v>
+      </c>
+      <c r="I35" s="4">
+        <f t="shared" si="22"/>
+        <v>30</v>
+      </c>
+      <c r="J35" s="4">
+        <f t="shared" si="23"/>
+        <v>62</v>
+      </c>
       <c r="K35" s="8"/>
       <c r="L35" s="5"/>
     </row>
     <row r="36" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
+      <c r="A36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="4">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="C36" s="4">
+        <f t="shared" si="19"/>
+        <v>-38</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="20"/>
+        <v>-46</v>
+      </c>
+      <c r="E36" s="4">
+        <v>70</v>
+      </c>
+      <c r="F36" s="4">
+        <v>62</v>
+      </c>
+      <c r="G36" s="4">
+        <v>108</v>
+      </c>
+      <c r="H36" s="4">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="I36" s="4">
+        <f t="shared" si="22"/>
+        <v>38</v>
+      </c>
+      <c r="J36" s="4">
+        <f t="shared" si="23"/>
+        <v>46</v>
+      </c>
       <c r="K36" s="8"/>
       <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
+      <c r="A37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="4">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="C37" s="4">
+        <f t="shared" si="19"/>
+        <v>-8</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="20"/>
+        <v>-16</v>
+      </c>
+      <c r="E37" s="4">
+        <v>38</v>
+      </c>
+      <c r="F37" s="4">
+        <v>30</v>
+      </c>
+      <c r="G37" s="4">
+        <v>46</v>
+      </c>
+      <c r="H37" s="4">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="I37" s="4">
+        <f t="shared" si="22"/>
+        <v>8</v>
+      </c>
+      <c r="J37" s="4">
+        <f t="shared" si="23"/>
+        <v>16</v>
+      </c>
       <c r="K37" s="8"/>
       <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
+      <c r="A38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="4">
+        <f t="shared" si="18"/>
+        <v>16</v>
+      </c>
+      <c r="C38" s="4">
+        <f t="shared" si="19"/>
+        <v>-16</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" si="20"/>
+        <v>-32</v>
+      </c>
+      <c r="E38" s="4">
+        <v>46</v>
+      </c>
+      <c r="F38" s="4">
+        <v>30</v>
+      </c>
+      <c r="G38" s="4">
+        <v>62</v>
+      </c>
+      <c r="H38" s="4">
+        <f t="shared" si="21"/>
+        <v>16</v>
+      </c>
+      <c r="I38" s="4">
+        <f t="shared" si="22"/>
+        <v>16</v>
+      </c>
+      <c r="J38" s="4">
+        <f t="shared" si="23"/>
+        <v>32</v>
+      </c>
       <c r="K38" s="8"/>
       <c r="L38" s="5"/>
     </row>
     <row r="39" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
+      <c r="A39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="4">
+        <f t="shared" si="18"/>
+        <v>22</v>
+      </c>
+      <c r="C39" s="4">
+        <f t="shared" si="19"/>
+        <v>-10</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="20"/>
+        <v>-32</v>
+      </c>
+      <c r="E39" s="4">
+        <v>108</v>
+      </c>
+      <c r="F39" s="4">
+        <v>86</v>
+      </c>
+      <c r="G39" s="4">
+        <v>118</v>
+      </c>
+      <c r="H39" s="4">
+        <f t="shared" si="21"/>
+        <v>22</v>
+      </c>
+      <c r="I39" s="4">
+        <f t="shared" si="22"/>
+        <v>10</v>
+      </c>
+      <c r="J39" s="4">
+        <f t="shared" si="23"/>
+        <v>32</v>
+      </c>
       <c r="K39" s="8"/>
       <c r="L39" s="5"/>
     </row>
     <row r="40" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
+      <c r="A40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="4">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="C40" s="4">
+        <f t="shared" si="19"/>
+        <v>-18</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" si="20"/>
+        <v>-26</v>
+      </c>
+      <c r="E40" s="4">
+        <v>98</v>
+      </c>
+      <c r="F40" s="4">
+        <v>90</v>
+      </c>
+      <c r="G40" s="4">
+        <v>116</v>
+      </c>
+      <c r="H40" s="4">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="I40" s="4">
+        <f t="shared" si="22"/>
+        <v>18</v>
+      </c>
+      <c r="J40" s="4">
+        <f t="shared" si="23"/>
+        <v>26</v>
+      </c>
       <c r="K40" s="8"/>
       <c r="L40" s="5"/>
     </row>
     <row r="41" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
+      <c r="A41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="4">
+        <f t="shared" si="18"/>
+        <v>-8</v>
+      </c>
+      <c r="C41" s="4">
+        <f t="shared" si="19"/>
+        <v>28</v>
+      </c>
+      <c r="D41" s="4">
+        <f t="shared" si="20"/>
+        <v>36</v>
+      </c>
+      <c r="E41" s="4">
+        <v>112</v>
+      </c>
+      <c r="F41" s="4">
+        <v>120</v>
+      </c>
+      <c r="G41" s="4">
+        <v>84</v>
+      </c>
+      <c r="H41" s="4">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="I41" s="4">
+        <f t="shared" si="22"/>
+        <v>28</v>
+      </c>
+      <c r="J41" s="4">
+        <f t="shared" si="23"/>
+        <v>36</v>
+      </c>
       <c r="K41" s="8"/>
       <c r="L41" s="5"/>
     </row>
     <row r="42" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
+      <c r="A42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="4">
+        <f t="shared" si="18"/>
+        <v>-14</v>
+      </c>
+      <c r="C42" s="4">
+        <f t="shared" si="19"/>
+        <v>68</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" si="20"/>
+        <v>82</v>
+      </c>
+      <c r="E42" s="4">
+        <v>106</v>
+      </c>
+      <c r="F42" s="4">
+        <v>120</v>
+      </c>
+      <c r="G42" s="4">
+        <v>38</v>
+      </c>
+      <c r="H42" s="4">
+        <f t="shared" si="21"/>
+        <v>14</v>
+      </c>
+      <c r="I42" s="4">
+        <f t="shared" si="22"/>
+        <v>68</v>
+      </c>
+      <c r="J42" s="4">
+        <f t="shared" si="23"/>
+        <v>82</v>
+      </c>
       <c r="K42" s="8"/>
       <c r="L42" s="5"/>
     </row>
     <row r="43" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
+      <c r="A43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="4">
+        <f t="shared" si="18"/>
+        <v>16</v>
+      </c>
+      <c r="C43" s="4">
+        <f t="shared" si="19"/>
+        <v>-16</v>
+      </c>
+      <c r="D43" s="4">
+        <f t="shared" si="20"/>
+        <v>-32</v>
+      </c>
+      <c r="E43" s="4">
+        <v>54</v>
+      </c>
+      <c r="F43" s="4">
+        <v>38</v>
+      </c>
+      <c r="G43" s="4">
+        <v>70</v>
+      </c>
+      <c r="H43" s="4">
+        <f t="shared" si="21"/>
+        <v>16</v>
+      </c>
+      <c r="I43" s="4">
+        <f t="shared" si="22"/>
+        <v>16</v>
+      </c>
+      <c r="J43" s="4">
+        <f t="shared" si="23"/>
+        <v>32</v>
+      </c>
       <c r="K43" s="8"/>
       <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
+      <c r="A44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="4">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="C44" s="4">
+        <f t="shared" si="19"/>
+        <v>-8</v>
+      </c>
+      <c r="D44" s="4">
+        <f t="shared" si="20"/>
+        <v>-16</v>
+      </c>
+      <c r="E44" s="4">
+        <v>62</v>
+      </c>
+      <c r="F44" s="4">
+        <v>54</v>
+      </c>
+      <c r="G44" s="4">
+        <v>70</v>
+      </c>
+      <c r="H44" s="4">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="I44" s="4">
+        <f t="shared" si="22"/>
+        <v>8</v>
+      </c>
+      <c r="J44" s="4">
+        <f t="shared" si="23"/>
+        <v>16</v>
+      </c>
       <c r="K44" s="8"/>
       <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
+      <c r="A45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="4">
+        <f t="shared" si="18"/>
+        <v>-12</v>
+      </c>
+      <c r="C45" s="4">
+        <f t="shared" si="19"/>
+        <v>22</v>
+      </c>
+      <c r="D45" s="4">
+        <f t="shared" si="20"/>
+        <v>34</v>
+      </c>
+      <c r="E45" s="4">
+        <v>108</v>
+      </c>
+      <c r="F45" s="4">
+        <v>120</v>
+      </c>
+      <c r="G45" s="4">
+        <v>86</v>
+      </c>
+      <c r="H45" s="4">
+        <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="I45" s="4">
+        <f t="shared" si="22"/>
+        <v>22</v>
+      </c>
+      <c r="J45" s="4">
+        <f t="shared" si="23"/>
+        <v>34</v>
+      </c>
       <c r="K45" s="8"/>
       <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
+      <c r="A46" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="4">
+        <f t="shared" si="18"/>
+        <v>16</v>
+      </c>
+      <c r="C46" s="4">
+        <f t="shared" si="19"/>
+        <v>-44</v>
+      </c>
+      <c r="D46" s="4">
+        <f t="shared" si="20"/>
+        <v>-60</v>
+      </c>
+      <c r="E46" s="4">
+        <v>46</v>
+      </c>
+      <c r="F46" s="4">
+        <v>30</v>
+      </c>
+      <c r="G46" s="4">
+        <v>90</v>
+      </c>
+      <c r="H46" s="4">
+        <f t="shared" si="21"/>
+        <v>16</v>
+      </c>
+      <c r="I46" s="4">
+        <f t="shared" si="22"/>
+        <v>44</v>
+      </c>
+      <c r="J46" s="4">
+        <f t="shared" si="23"/>
+        <v>60</v>
+      </c>
       <c r="K46" s="8"/>
       <c r="L46" s="5"/>
     </row>
     <row r="47" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
+      <c r="A47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="4">
+        <f t="shared" si="18"/>
+        <v>-20</v>
+      </c>
+      <c r="C47" s="4">
+        <f t="shared" si="19"/>
+        <v>16</v>
+      </c>
+      <c r="D47" s="4">
+        <f t="shared" si="20"/>
+        <v>36</v>
+      </c>
+      <c r="E47" s="4">
+        <v>98</v>
+      </c>
+      <c r="F47" s="4">
+        <v>118</v>
+      </c>
+      <c r="G47" s="4">
+        <v>82</v>
+      </c>
+      <c r="H47" s="4">
+        <f t="shared" si="21"/>
+        <v>20</v>
+      </c>
+      <c r="I47" s="4">
+        <f t="shared" si="22"/>
+        <v>16</v>
+      </c>
+      <c r="J47" s="4">
+        <f t="shared" si="23"/>
+        <v>36</v>
+      </c>
       <c r="K47" s="8"/>
       <c r="L47" s="5"/>
     </row>
     <row r="48" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
+      <c r="A48" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="4">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="C48" s="4">
+        <f t="shared" si="19"/>
+        <v>-54</v>
+      </c>
+      <c r="D48" s="4">
+        <f t="shared" si="20"/>
+        <v>-62</v>
+      </c>
+      <c r="E48" s="4">
+        <v>38</v>
+      </c>
+      <c r="F48" s="4">
+        <v>30</v>
+      </c>
+      <c r="G48" s="4">
+        <v>92</v>
+      </c>
+      <c r="H48" s="4">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="I48" s="4">
+        <f t="shared" si="22"/>
+        <v>54</v>
+      </c>
+      <c r="J48" s="4">
+        <f t="shared" si="23"/>
+        <v>62</v>
+      </c>
       <c r="K48" s="8"/>
       <c r="L48" s="5"/>
     </row>
     <row r="49" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
+      <c r="A49" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="4">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="C49" s="4">
+        <f t="shared" si="19"/>
+        <v>-52</v>
+      </c>
+      <c r="D49" s="4">
+        <f t="shared" si="20"/>
+        <v>-60</v>
+      </c>
+      <c r="E49" s="4">
+        <v>62</v>
+      </c>
+      <c r="F49" s="4">
+        <v>54</v>
+      </c>
+      <c r="G49" s="4">
+        <v>114</v>
+      </c>
+      <c r="H49" s="4">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="I49" s="4">
+        <f t="shared" si="22"/>
+        <v>52</v>
+      </c>
+      <c r="J49" s="4">
+        <f t="shared" si="23"/>
+        <v>60</v>
+      </c>
       <c r="K49" s="8"/>
       <c r="L49" s="5"/>
     </row>

</xml_diff>